<commit_message>
Look at ALT soln by Bo
</commit_message>
<xml_diff>
--- a/CH-86 KNN Missing values.xlsx
+++ b/CH-86 KNN Missing values.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B39E050-0C21-4AF6-B514-2E0BB5133EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CFCC86-B1F2-48AD-92F4-23FF8B332BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$C$2:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$C$2:$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -57,6 +81,12 @@
   </si>
   <si>
     <t>Row ID</t>
+  </si>
+  <si>
+    <t>Bo Solution</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7220895320518410240/</t>
   </si>
 </sst>
 </file>
@@ -914,11 +944,40 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{856BC94D-D04D-40E4-A52A-204328FB8957}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{7E0E9D39-FB08-4512-90D1-72A57D565F40}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -1456,4 +1515,677 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C7865D-C930-4F5F-B352-C568D33565EE}">
+  <dimension ref="C1:Q75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.88671875" customWidth="1"/>
+    <col min="3" max="4" width="9.6640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="8" width="5.77734375" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:17" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="3:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7">
+        <v>89</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>11</v>
+      </c>
+      <c r="K3" s="7">
+        <v>12</v>
+      </c>
+      <c r="L3" s="7">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>32</v>
+      </c>
+      <c r="E4" s="7">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7">
+        <v>78</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
+      <c r="J4" s="7">
+        <v>32</v>
+      </c>
+      <c r="K4" s="7">
+        <v>36</v>
+      </c>
+      <c r="L4" s="7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>78</v>
+      </c>
+      <c r="E5" s="7">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7">
+        <v>78</v>
+      </c>
+      <c r="K5" s="7">
+        <v>50</v>
+      </c>
+      <c r="L5" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>65</v>
+      </c>
+      <c r="E6" s="7">
+        <v>67</v>
+      </c>
+      <c r="F6" s="7">
+        <v>94</v>
+      </c>
+      <c r="I6" s="7">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>65</v>
+      </c>
+      <c r="K6" s="7">
+        <v>67</v>
+      </c>
+      <c r="L6" s="7">
+        <v>94</v>
+      </c>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7">
+        <v>94</v>
+      </c>
+      <c r="E7" s="7">
+        <v>84</v>
+      </c>
+      <c r="F7" s="7">
+        <v>82</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>94</v>
+      </c>
+      <c r="K7" s="7">
+        <v>84</v>
+      </c>
+      <c r="L7" s="7">
+        <v>82</v>
+      </c>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>57</v>
+      </c>
+      <c r="E8" s="7">
+        <v>68</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="I8" s="7">
+        <v>6</v>
+      </c>
+      <c r="J8" s="7">
+        <v>57</v>
+      </c>
+      <c r="K8" s="7">
+        <v>68</v>
+      </c>
+      <c r="L8" s="8">
+        <v>52</v>
+      </c>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C9" s="7">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7">
+        <v>12</v>
+      </c>
+      <c r="I9" s="7">
+        <v>7</v>
+      </c>
+      <c r="J9" s="8">
+        <v>55</v>
+      </c>
+      <c r="K9" s="7">
+        <v>30</v>
+      </c>
+      <c r="L9" s="7">
+        <v>12</v>
+      </c>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7">
+        <v>40</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="I10" s="7">
+        <v>8</v>
+      </c>
+      <c r="J10" s="7">
+        <v>40</v>
+      </c>
+      <c r="K10" s="8">
+        <v>51.5</v>
+      </c>
+      <c r="L10" s="8">
+        <v>86</v>
+      </c>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7">
+        <v>10</v>
+      </c>
+      <c r="I11" s="7">
+        <v>9</v>
+      </c>
+      <c r="J11" s="7">
+        <v>34</v>
+      </c>
+      <c r="K11" s="8">
+        <v>44</v>
+      </c>
+      <c r="L11" s="7">
+        <v>10</v>
+      </c>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7">
+        <v>70</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="I12" s="7">
+        <v>10</v>
+      </c>
+      <c r="J12" s="7">
+        <v>10</v>
+      </c>
+      <c r="K12" s="7">
+        <v>70</v>
+      </c>
+      <c r="L12" s="8">
+        <v>86</v>
+      </c>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N15" s="6"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" cm="1">
+        <f t="array" ref="C16:E25">_xlfn.LET(
+    _xlpm.n, D3:F12,
+    _xlpm.k, _xlfn.TAKE(_xlpm.n, 5),
+    _xlfn.MAP(
+        _xlpm.n,
+        _xlfn.LAMBDA(_xlpm.v,
+            _xlfn.LET(
+                _xlpm.a, D3:_xlpm.v,
+                _xlpm.r, INDEX(_xlpm.n, ROWS(_xlpm.a), ),
+                IF(
+                    _xlpm.v,
+                    _xlpm.v,
+                    AVERAGE(
+                        _xlfn.TAKE(
+                            _xlfn.SORTBY(
+                                INDEX(_xlpm.k, , COLUMNS(_xlpm.a)),
+                                _xlfn.BYROW(_xlfn._xlws.FILTER((_xlpm.k - _xlpm.r) ^ 2, _xlpm.r), _xleta.SUM)
+                            ),
+                            2
+                        )
+                    )
+                )
+            )
+        )
+    )
+)</f>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>89</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C17" s="3">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3">
+        <v>36</v>
+      </c>
+      <c r="E17">
+        <v>78</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C18" s="3">
+        <v>78</v>
+      </c>
+      <c r="D18" s="3">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C19" s="3">
+        <v>65</v>
+      </c>
+      <c r="D19" s="3">
+        <v>67</v>
+      </c>
+      <c r="E19">
+        <v>94</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C20" s="3">
+        <v>94</v>
+      </c>
+      <c r="D20" s="3">
+        <v>84</v>
+      </c>
+      <c r="E20">
+        <v>82</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <v>57</v>
+      </c>
+      <c r="D21" s="3">
+        <v>68</v>
+      </c>
+      <c r="E21">
+        <v>52</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <v>55</v>
+      </c>
+      <c r="D22" s="3">
+        <v>30</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C23" s="3">
+        <v>40</v>
+      </c>
+      <c r="D23" s="3">
+        <v>51.5</v>
+      </c>
+      <c r="E23">
+        <v>86</v>
+      </c>
+      <c r="N23" s="6"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C24" s="3">
+        <v>34</v>
+      </c>
+      <c r="D24" s="3">
+        <v>43</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C25" s="3">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3">
+        <v>70</v>
+      </c>
+      <c r="E25">
+        <v>86</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N26" s="6"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N27" s="6"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N28" s="6"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N29" s="6"/>
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N30" s="6"/>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N31" s="1"/>
+      <c r="Q31" s="1"/>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="N32" s="1"/>
+      <c r="Q32" s="1"/>
+    </row>
+    <row r="33" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N33" s="1"/>
+      <c r="Q33" s="1"/>
+    </row>
+    <row r="34" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N34" s="1"/>
+      <c r="Q34" s="1"/>
+    </row>
+    <row r="35" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N35" s="1"/>
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N36" s="1"/>
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="37" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N37" s="1"/>
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N38" s="1"/>
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N39" s="1"/>
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N40" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q43" s="1"/>
+    </row>
+    <row r="44" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q45" s="1"/>
+    </row>
+    <row r="46" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q46" s="1"/>
+    </row>
+    <row r="47" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q47" s="1"/>
+    </row>
+    <row r="48" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q48" s="1"/>
+    </row>
+    <row r="49" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q50" s="1"/>
+    </row>
+    <row r="51" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q51" s="1"/>
+    </row>
+    <row r="52" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q52" s="1"/>
+    </row>
+    <row r="53" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q53" s="1"/>
+    </row>
+    <row r="54" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q54" s="1"/>
+    </row>
+    <row r="55" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q55" s="1"/>
+    </row>
+    <row r="56" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q56" s="1"/>
+    </row>
+    <row r="57" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q57" s="1"/>
+    </row>
+    <row r="58" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q58" s="1"/>
+    </row>
+    <row r="59" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q59" s="1"/>
+    </row>
+    <row r="60" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q60" s="1"/>
+    </row>
+    <row r="61" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q61" s="1"/>
+    </row>
+    <row r="62" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q62" s="1"/>
+    </row>
+    <row r="63" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q63" s="1"/>
+    </row>
+    <row r="64" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q64" s="1"/>
+    </row>
+    <row r="65" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q65" s="1"/>
+    </row>
+    <row r="66" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q66" s="1"/>
+    </row>
+    <row r="67" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q67" s="1"/>
+    </row>
+    <row r="68" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q68" s="1"/>
+    </row>
+    <row r="69" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q69" s="1"/>
+    </row>
+    <row r="70" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q70" s="1"/>
+    </row>
+    <row r="71" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q71" s="1"/>
+    </row>
+    <row r="72" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q72" s="1"/>
+    </row>
+    <row r="73" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q73" s="1"/>
+    </row>
+    <row r="74" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q74" s="1"/>
+    </row>
+    <row r="75" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q75" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E0E9D39-FB08-4512-90D1-72A57D565F40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Going through Bo solution
</commit_message>
<xml_diff>
--- a/CH-86 KNN Missing values.xlsx
+++ b/CH-86 KNN Missing values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CFCC86-B1F2-48AD-92F4-23FF8B332BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A9DCE-3FE8-4438-A109-B33471B7D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1522,7 +1522,7 @@
   <dimension ref="C1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Working on my EDA. I just duplicated the solution manually
</commit_message>
<xml_diff>
--- a/CH-86 KNN Missing values.xlsx
+++ b/CH-86 KNN Missing values.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A9DCE-3FE8-4438-A109-B33471B7D60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71033782-9BD3-4FF9-AF2B-F1E394A069B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="EDA" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$C$2:$C$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EDA!$C$2:$C$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$C$2:$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -946,7 +948,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="422" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -977,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,7 +1188,10 @@
       <c r="L8" s="8">
         <v>52</v>
       </c>
-      <c r="N8" s="5"/>
+      <c r="N8" s="5" cm="1">
+        <f t="array" ref="N8">SUM((J3:J7-J8)^2)</f>
+        <v>4615</v>
+      </c>
     </row>
     <row r="9" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C9" s="7">
@@ -1521,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C7865D-C930-4F5F-B352-C568D33565EE}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,7 +1803,7 @@
         <v>34</v>
       </c>
       <c r="K11" s="8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="7">
         <v>10</v>
@@ -2178,6 +2183,806 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA172D4-4032-4CA9-BD58-19DE41874FD9}">
+  <dimension ref="C1:Q75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="2.88671875" customWidth="1"/>
+    <col min="3" max="4" width="9.6640625" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="8" width="5.77734375" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:17" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="3:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7">
+        <v>89</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>11</v>
+      </c>
+      <c r="K3" s="7">
+        <v>12</v>
+      </c>
+      <c r="L3" s="7">
+        <v>89</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <f>($J$8-J3)^2+($K$8-K3)^2</f>
+        <v>5252</v>
+      </c>
+      <c r="O3" s="2" cm="1">
+        <f t="array" ref="O3:P4">_xlfn.TAKE(_xlfn._xlws.SORT(M3:N7,2),2)</f>
+        <v>4</v>
+      </c>
+      <c r="P3" s="2">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="2" cm="1">
+        <f t="array" ref="Q3">AVERAGE(INDEX(L3:L7,O3:O4))</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>32</v>
+      </c>
+      <c r="E4" s="7">
+        <v>36</v>
+      </c>
+      <c r="F4" s="7">
+        <v>78</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2</v>
+      </c>
+      <c r="J4" s="7">
+        <v>32</v>
+      </c>
+      <c r="K4" s="7">
+        <v>36</v>
+      </c>
+      <c r="L4" s="7">
+        <v>78</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N7" si="0">($J$8-J4)^2+($K$8-K4)^2</f>
+        <v>1649</v>
+      </c>
+      <c r="O4" s="2">
+        <v>3</v>
+      </c>
+      <c r="P4" s="2">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>78</v>
+      </c>
+      <c r="E5" s="7">
+        <v>50</v>
+      </c>
+      <c r="F5" s="7">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7">
+        <v>78</v>
+      </c>
+      <c r="K5" s="7">
+        <v>50</v>
+      </c>
+      <c r="L5" s="7">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>765</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>65</v>
+      </c>
+      <c r="E6" s="7">
+        <v>67</v>
+      </c>
+      <c r="F6" s="7">
+        <v>94</v>
+      </c>
+      <c r="I6" s="7">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7">
+        <v>65</v>
+      </c>
+      <c r="K6" s="7">
+        <v>67</v>
+      </c>
+      <c r="L6" s="7">
+        <v>94</v>
+      </c>
+      <c r="M6" s="2">
+        <v>4</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7">
+        <v>94</v>
+      </c>
+      <c r="E7" s="7">
+        <v>84</v>
+      </c>
+      <c r="F7" s="7">
+        <v>82</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>94</v>
+      </c>
+      <c r="K7" s="7">
+        <v>84</v>
+      </c>
+      <c r="L7" s="7">
+        <v>82</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>57</v>
+      </c>
+      <c r="E8" s="7">
+        <v>68</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="I8" s="7">
+        <v>6</v>
+      </c>
+      <c r="J8" s="7">
+        <v>57</v>
+      </c>
+      <c r="K8" s="7">
+        <v>68</v>
+      </c>
+      <c r="L8" s="8">
+        <v>52</v>
+      </c>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C9" s="7">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7">
+        <v>12</v>
+      </c>
+      <c r="I9" s="7">
+        <v>7</v>
+      </c>
+      <c r="J9" s="8">
+        <v>55</v>
+      </c>
+      <c r="K9" s="7">
+        <v>30</v>
+      </c>
+      <c r="L9" s="7">
+        <v>12</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" cm="1">
+        <f t="array" ref="N9:N13">(K3:K7-K9)^2+(L3:L7-L9)^2</f>
+        <v>6253</v>
+      </c>
+      <c r="O9" s="2" cm="1">
+        <f t="array" ref="O9:P10">_xlfn.TAKE(_xlfn._xlws.SORT(M9:N13,2),2)</f>
+        <v>3</v>
+      </c>
+      <c r="P9" s="2">
+        <v>404</v>
+      </c>
+      <c r="Q9" s="2" cm="1">
+        <f t="array" ref="Q9">AVERAGE(INDEX(J3:J8,O9:O10))</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7">
+        <v>40</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="I10" s="7">
+        <v>8</v>
+      </c>
+      <c r="J10" s="7">
+        <v>40</v>
+      </c>
+      <c r="K10" s="8">
+        <v>51.5</v>
+      </c>
+      <c r="L10" s="8">
+        <v>86</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>4392</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2</v>
+      </c>
+      <c r="P10" s="2">
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7">
+        <v>34</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7">
+        <v>10</v>
+      </c>
+      <c r="I11" s="7">
+        <v>9</v>
+      </c>
+      <c r="J11" s="7">
+        <v>34</v>
+      </c>
+      <c r="K11" s="8">
+        <v>43</v>
+      </c>
+      <c r="L11" s="7">
+        <v>10</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3</v>
+      </c>
+      <c r="N11" s="2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7">
+        <v>70</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="I12" s="7">
+        <v>10</v>
+      </c>
+      <c r="J12" s="7">
+        <v>10</v>
+      </c>
+      <c r="K12" s="7">
+        <v>70</v>
+      </c>
+      <c r="L12" s="8">
+        <v>86</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4</v>
+      </c>
+      <c r="N12" s="2">
+        <v>8093</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <v>7816</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="M14" s="2"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6" cm="1">
+        <f t="array" ref="N15:N19">(J3:J7-J11)^2+(L3:L7-L11)^2</f>
+        <v>6770</v>
+      </c>
+      <c r="O15" cm="1">
+        <f t="array" ref="O15:P16">_xlfn.TAKE(_xlfn._xlws.SORT(M15:N19,2),2)</f>
+        <v>3</v>
+      </c>
+      <c r="P15">
+        <v>1936</v>
+      </c>
+      <c r="Q15" s="2" cm="1">
+        <f t="array" ref="Q15">AVERAGE(INDEX(K3:K8,O15:O16))</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="M16" s="2">
+        <v>2</v>
+      </c>
+      <c r="N16" s="6">
+        <v>4628</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>4628</v>
+      </c>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M17" s="2">
+        <v>3</v>
+      </c>
+      <c r="N17" s="6">
+        <v>1936</v>
+      </c>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M18" s="2">
+        <v>4</v>
+      </c>
+      <c r="N18" s="6">
+        <v>8017</v>
+      </c>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M19" s="2">
+        <v>5</v>
+      </c>
+      <c r="N19" s="6">
+        <v>8784</v>
+      </c>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="N20" s="6"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="6" cm="1">
+        <f t="array" ref="N21:N25">(J3:J7-J12)^2+(K3:K7-K12)^2</f>
+        <v>3365</v>
+      </c>
+      <c r="O21" cm="1">
+        <f t="array" ref="O21:P22">_xlfn.TAKE(_xlfn._xlws.SORT(M21:N25,2),2)</f>
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>1640</v>
+      </c>
+      <c r="Q21" s="2" cm="1">
+        <f t="array" ref="Q21">AVERAGE(INDEX(L3:L7,O21:O22))</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M22" s="2">
+        <v>2</v>
+      </c>
+      <c r="N22" s="6">
+        <v>1640</v>
+      </c>
+      <c r="O22">
+        <v>4</v>
+      </c>
+      <c r="P22">
+        <v>3034</v>
+      </c>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M23" s="2">
+        <v>3</v>
+      </c>
+      <c r="N23" s="6">
+        <v>5024</v>
+      </c>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M24" s="2">
+        <v>4</v>
+      </c>
+      <c r="N24" s="6">
+        <v>3034</v>
+      </c>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M25" s="2">
+        <v>5</v>
+      </c>
+      <c r="N25" s="6">
+        <v>7252</v>
+      </c>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="N26" s="6"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M27" s="2">
+        <v>1</v>
+      </c>
+      <c r="N27" s="6" cm="1">
+        <f t="array" ref="N27:N31">(J3:J7-J10)^2</f>
+        <v>841</v>
+      </c>
+      <c r="O27" cm="1">
+        <f t="array" ref="O27:P28">_xlfn.TAKE(_xlfn._xlws.SORT(M27:N31,2),2)</f>
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>64</v>
+      </c>
+      <c r="Q27" s="2" cm="1">
+        <f t="array" ref="Q27">AVERAGE(INDEX(K3:K7,O27:O28))</f>
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="28" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M28" s="2">
+        <v>2</v>
+      </c>
+      <c r="N28" s="6">
+        <v>64</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+      <c r="P28">
+        <v>625</v>
+      </c>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M29" s="2">
+        <v>3</v>
+      </c>
+      <c r="N29" s="6">
+        <v>1444</v>
+      </c>
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M30" s="2">
+        <v>4</v>
+      </c>
+      <c r="N30" s="6">
+        <v>625</v>
+      </c>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M31" s="2">
+        <v>5</v>
+      </c>
+      <c r="N31" s="6">
+        <v>2916</v>
+      </c>
+      <c r="Q31" s="1"/>
+    </row>
+    <row r="32" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="N32" s="1"/>
+      <c r="Q32" s="1"/>
+    </row>
+    <row r="33" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M33" s="2">
+        <v>1</v>
+      </c>
+      <c r="N33" s="6" cm="1">
+        <f t="array" ref="N33:N37">(J3:J7-J10)^2</f>
+        <v>841</v>
+      </c>
+      <c r="O33" cm="1">
+        <f t="array" ref="O33:P34">_xlfn.TAKE(_xlfn._xlws.SORT(M33:N37,2),2)</f>
+        <v>2</v>
+      </c>
+      <c r="P33">
+        <v>64</v>
+      </c>
+      <c r="Q33" s="2" cm="1">
+        <f t="array" ref="Q33">AVERAGE(INDEX(L3:L7,O33:O34))</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M34" s="2">
+        <v>2</v>
+      </c>
+      <c r="N34" s="6">
+        <v>64</v>
+      </c>
+      <c r="O34">
+        <v>4</v>
+      </c>
+      <c r="P34">
+        <v>625</v>
+      </c>
+      <c r="Q34" s="1"/>
+    </row>
+    <row r="35" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M35" s="2">
+        <v>3</v>
+      </c>
+      <c r="N35" s="6">
+        <v>1444</v>
+      </c>
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M36" s="2">
+        <v>4</v>
+      </c>
+      <c r="N36" s="6">
+        <v>625</v>
+      </c>
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="37" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="M37" s="2">
+        <v>5</v>
+      </c>
+      <c r="N37" s="6">
+        <v>2916</v>
+      </c>
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="N38" s="1"/>
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="N39" s="1"/>
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="N40" s="1"/>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q43" s="1"/>
+    </row>
+    <row r="44" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q45" s="1"/>
+    </row>
+    <row r="46" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q46" s="1"/>
+    </row>
+    <row r="47" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q47" s="1"/>
+    </row>
+    <row r="48" spans="13:17" x14ac:dyDescent="0.3">
+      <c r="Q48" s="1"/>
+    </row>
+    <row r="49" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q49" s="1"/>
+    </row>
+    <row r="50" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q50" s="1"/>
+    </row>
+    <row r="51" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q51" s="1"/>
+    </row>
+    <row r="52" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q52" s="1"/>
+    </row>
+    <row r="53" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q53" s="1"/>
+    </row>
+    <row r="54" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q54" s="1"/>
+    </row>
+    <row r="55" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q55" s="1"/>
+    </row>
+    <row r="56" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q56" s="1"/>
+    </row>
+    <row r="57" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q57" s="1"/>
+    </row>
+    <row r="58" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q58" s="1"/>
+    </row>
+    <row r="59" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q59" s="1"/>
+    </row>
+    <row r="60" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q60" s="1"/>
+    </row>
+    <row r="61" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q61" s="1"/>
+    </row>
+    <row r="62" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q62" s="1"/>
+    </row>
+    <row r="63" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q63" s="1"/>
+    </row>
+    <row r="64" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q64" s="1"/>
+    </row>
+    <row r="65" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q65" s="1"/>
+    </row>
+    <row r="66" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q66" s="1"/>
+    </row>
+    <row r="67" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q67" s="1"/>
+    </row>
+    <row r="68" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q68" s="1"/>
+    </row>
+    <row r="69" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q69" s="1"/>
+    </row>
+    <row r="70" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q70" s="1"/>
+    </row>
+    <row r="71" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q71" s="1"/>
+    </row>
+    <row r="72" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q72" s="1"/>
+    </row>
+    <row r="73" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q73" s="1"/>
+    </row>
+    <row r="74" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q74" s="1"/>
+    </row>
+    <row r="75" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q75" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>

</xml_diff>

<commit_message>
Well, I believe I understand Bo's solution. Brilliant.
</commit_message>
<xml_diff>
--- a/CH-86 KNN Missing values.xlsx
+++ b/CH-86 KNN Missing values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71033782-9BD3-4FF9-AF2B-F1E394A069B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF00F44-CB20-4D29-8A88-0556261CA13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -966,6 +966,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1526,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C7865D-C930-4F5F-B352-C568D33565EE}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2187,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA172D4-4032-4CA9-BD58-19DE41874FD9}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
I looked closer at the filter function. Beautiful.
</commit_message>
<xml_diff>
--- a/CH-86 KNN Missing values.xlsx
+++ b/CH-86 KNN Missing values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF00F44-CB20-4D29-8A88-0556261CA13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531B0E4-9480-4A14-973A-0826AFBDE713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7220895320518410240/</t>
+  </si>
+  <si>
+    <t>Excellent filter technique</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -194,6 +197,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C7865D-C930-4F5F-B352-C568D33565EE}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2190,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA172D4-4032-4CA9-BD58-19DE41874FD9}">
   <dimension ref="C1:Q75"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2620,6 +2626,9 @@
       </c>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C16" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="M16" s="2">
         <v>2</v>
       </c>
@@ -2634,7 +2643,7 @@
       </c>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M17" s="2">
         <v>3</v>
       </c>
@@ -2643,7 +2652,14 @@
       </c>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" cm="1">
+        <f t="array" ref="C18:D22">_xlfn._xlws.FILTER(D3:F7,D8:F8)</f>
+        <v>11</v>
+      </c>
+      <c r="D18" s="3">
+        <v>12</v>
+      </c>
       <c r="M18" s="2">
         <v>4</v>
       </c>
@@ -2652,7 +2668,13 @@
       </c>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C19" s="3">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3">
+        <v>36</v>
+      </c>
       <c r="M19" s="2">
         <v>5</v>
       </c>
@@ -2661,11 +2683,23 @@
       </c>
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C20" s="3">
+        <v>78</v>
+      </c>
+      <c r="D20" s="3">
+        <v>50</v>
+      </c>
       <c r="N20" s="6"/>
       <c r="Q20" s="1"/>
     </row>
-    <row r="21" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="3">
+        <v>65</v>
+      </c>
+      <c r="D21" s="3">
+        <v>67</v>
+      </c>
       <c r="M21" s="2">
         <v>1</v>
       </c>
@@ -2685,7 +2719,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C22" s="3">
+        <v>94</v>
+      </c>
+      <c r="D22" s="3">
+        <v>84</v>
+      </c>
       <c r="M22" s="2">
         <v>2</v>
       </c>
@@ -2700,7 +2740,7 @@
       </c>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M23" s="2">
         <v>3</v>
       </c>
@@ -2709,7 +2749,7 @@
       </c>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M24" s="2">
         <v>4</v>
       </c>
@@ -2718,7 +2758,7 @@
       </c>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M25" s="2">
         <v>5</v>
       </c>
@@ -2727,11 +2767,11 @@
       </c>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
       <c r="N26" s="6"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M27" s="2">
         <v>1</v>
       </c>
@@ -2751,7 +2791,7 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="28" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M28" s="2">
         <v>2</v>
       </c>
@@ -2766,7 +2806,7 @@
       </c>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M29" s="2">
         <v>3</v>
       </c>
@@ -2775,7 +2815,7 @@
       </c>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M30" s="2">
         <v>4</v>
       </c>
@@ -2784,7 +2824,7 @@
       </c>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
       <c r="M31" s="2">
         <v>5</v>
       </c>
@@ -2793,7 +2833,7 @@
       </c>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="13:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:17" x14ac:dyDescent="0.3">
       <c r="N32" s="1"/>
       <c r="Q32" s="1"/>
     </row>

</xml_diff>